<commit_message>
feat: add all pwm pins in a func for easy use of the lib
</commit_message>
<xml_diff>
--- a/ATmega2560_Apps/.Resources/ATmega2560_Pinout/ATmega2560_Pinout.xlsx
+++ b/ATmega2560_Apps/.Resources/ATmega2560_Pinout/ATmega2560_Pinout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub_Projects\Embedded_Apps\ATmega2560_Apps\.Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub_Projects\Embedded_Apps\ATmega2560_Apps\.Resources\ATmega2560_Pinout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273ADD90-8CBC-45EC-89F6-812C9C33E7C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1513A672-4B72-435E-89B5-93C76AC1A570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="696" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -888,8 +888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -962,7 +962,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -973,7 +973,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -984,7 +984,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -993,7 +993,7 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" ht="98.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="98.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1196,7 +1196,7 @@
       </c>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1205,7 +1205,7 @@
       </c>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -1428,7 +1428,7 @@
       </c>
       <c r="C50" s="3"/>
     </row>
-    <row r="51" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -1602,7 +1602,7 @@
       </c>
       <c r="C66" s="3"/>
     </row>
-    <row r="67" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="C67" s="3"/>
     </row>
-    <row r="68" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -1620,7 +1620,7 @@
       </c>
       <c r="C68" s="3"/>
     </row>
-    <row r="69" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="C69" s="3"/>
     </row>
-    <row r="70" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C70" s="3"/>
     </row>
-    <row r="71" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="49.2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="73.8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>98</v>
       </c>

</xml_diff>